<commit_message>
I modify the "1año" to "1 año" text
</commit_message>
<xml_diff>
--- a/datasets/tabla_adulto_equiv.xlsx
+++ b/datasets/tabla_adulto_equiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pupih\Desktop\EPH_usu_1_Trim_2019_xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronny\Documents\GitHub\big-data-tp2\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E962F3C-29E4-4745-A82B-33515FD15C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3389BE-1649-415B-898E-C871D7FD89A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de adulo equivalente" sheetId="7" r:id="rId1"/>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Menor de 1 año</t>
-  </si>
-  <si>
-    <t>1año</t>
   </si>
   <si>
     <t>2 años</t>
@@ -146,11 +143,14 @@
   <si>
     <t>Hogar 3: de cinco integrantes, constituido por una pareja de un varón y una mujer, ambos de 30 años, y tres hijos de 5, 3 y 1 año. En total, el hogar suma 3,25 adultos equivalentes</t>
   </si>
+  <si>
+    <t>1 año</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +301,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -339,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,9 +379,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,26 +414,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,26 +449,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -658,14 +624,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -674,7 +640,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -716,7 +682,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6">
         <v>0.37</v>
@@ -727,7 +693,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="6">
         <v>0.46</v>
@@ -738,7 +704,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="6">
         <v>0.51</v>
@@ -749,7 +715,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="6">
         <v>0.55000000000000004</v>
@@ -760,7 +726,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6">
         <v>0.6</v>
@@ -771,7 +737,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="6">
         <v>0.64</v>
@@ -782,7 +748,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="6">
         <v>0.66</v>
@@ -793,7 +759,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6">
         <v>0.68</v>
@@ -804,7 +770,7 @@
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="7">
         <v>0.69</v>
@@ -815,7 +781,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="6">
         <v>0.7</v>
@@ -826,7 +792,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6">
         <v>0.72</v>
@@ -837,7 +803,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="6">
         <v>0.74</v>
@@ -848,7 +814,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="6">
         <v>0.76</v>
@@ -859,7 +825,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="6">
         <v>0.76</v>
@@ -870,7 +836,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="6">
         <v>0.77</v>
@@ -881,7 +847,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="6">
         <v>0.77</v>
@@ -892,7 +858,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6">
         <v>0.77</v>
@@ -903,7 +869,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="6">
         <v>0.76</v>
@@ -914,7 +880,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="6">
         <v>0.77</v>
@@ -925,7 +891,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="6">
         <v>0.76</v>
@@ -936,7 +902,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="6">
         <v>0.67</v>
@@ -947,7 +913,7 @@
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="9">
         <v>0.63</v>
@@ -959,7 +925,7 @@
     <row r="29" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -974,7 +940,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -1002,7 +968,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -1030,7 +996,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1051,7 +1017,7 @@
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -1065,7 +1031,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>